<commit_message>
updating all files and metadata to test XML creation process
</commit_message>
<xml_diff>
--- a/data-raw/FISHBIO_submission/FISHBIO_PIT_detection_metadata.xlsx
+++ b/data-raw/FISHBIO_submission/FISHBIO_PIT_detection_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin Cain\Documents\Git\CVPIA\data-stewardship\fishbio-stanislaus-o.mykiss\data-raw\FISHBIO submission\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddeerubenson/Documents/git/fishbio-stanislaus-o.mykiss/data-raw/FISHBIO_submission/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E5C948-F883-4A5B-8C18-6E2631270E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1CADFE7-E966-A646-B072-4E2B0A2D22DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="834" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28520" windowHeight="15740" tabRatio="834" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="attribute" sheetId="9" r:id="rId11"/>
     <sheet name="code_definitions" sheetId="10" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -371,9 +371,6 @@
     <t>comments</t>
   </si>
   <si>
-    <t>rbt</t>
-  </si>
-  <si>
     <t>Rainbow trout/Steelhead</t>
   </si>
   <si>
@@ -417,6 +414,9 @@
   </si>
   <si>
     <t>Any additional comments describing the passage record</t>
+  </si>
+  <si>
+    <t>RBT</t>
   </si>
 </sst>
 </file>
@@ -912,12 +912,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.375" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -928,7 +928,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>90</v>
       </c>
@@ -957,16 +957,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.625" customWidth="1"/>
-    <col min="2" max="2" width="20.375" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="9" max="9" width="10.375" customWidth="1"/>
-    <col min="10" max="10" width="32.625" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" customWidth="1"/>
+    <col min="10" max="10" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -998,7 +998,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>84</v>
       </c>
@@ -1020,29 +1020,29 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="19.625" style="2"/>
-    <col min="3" max="3" width="13.125" style="10" customWidth="1"/>
+    <col min="1" max="2" width="19.6640625" style="2"/>
+    <col min="3" max="3" width="13.1640625" style="10" customWidth="1"/>
     <col min="4" max="4" width="17.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="5.375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="12.125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="14.125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="5.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" style="10" customWidth="1"/>
     <col min="11" max="11" width="16" style="2" customWidth="1"/>
-    <col min="12" max="12" width="17.625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="10.625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="13.625" style="2" customWidth="1"/>
-    <col min="15" max="1022" width="19.625" style="2"/>
-    <col min="1023" max="1025" width="8.375" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" style="2" customWidth="1"/>
+    <col min="15" max="1022" width="19.6640625" style="2"/>
+    <col min="1023" max="1025" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1022" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1022" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>39</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:1022" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1022" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>101</v>
       </c>
@@ -1106,13 +1106,13 @@
         <v>86</v>
       </c>
       <c r="M2" s="14">
-        <v>38361</v>
+        <v>44650</v>
       </c>
       <c r="N2" s="14">
         <v>44656</v>
       </c>
     </row>
-    <row r="3" spans="1:1022" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1022" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>102</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:1022" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1022" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>103</v>
       </c>
@@ -1146,12 +1146,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:1022" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1022" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>88</v>
@@ -1160,12 +1160,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:1022" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1022" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>105</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>88</v>
@@ -1174,12 +1174,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:1022" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1022" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>106</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="15" t="s">
@@ -1187,7 +1187,7 @@
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
@@ -2206,12 +2206,12 @@
       <c r="AMG7" s="15"/>
       <c r="AMH7" s="15"/>
     </row>
-    <row r="8" spans="1:1022" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1022" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>85</v>
@@ -2232,12 +2232,12 @@
         <v>44550</v>
       </c>
     </row>
-    <row r="9" spans="1:1022" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1022" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>108</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>88</v>
@@ -2246,28 +2246,28 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:1022" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1022" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>109</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="H10" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="G10" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="H10" s="6" t="s">
+      <c r="I10" s="15" t="s">
         <v>124</v>
-      </c>
-      <c r="I10" s="15" t="s">
-        <v>125</v>
       </c>
       <c r="J10" s="16"/>
       <c r="K10" s="15"/>
@@ -2279,12 +2279,12 @@
         <v>480</v>
       </c>
     </row>
-    <row r="11" spans="1:1022" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1022" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="15" t="s">
@@ -2328,17 +2328,17 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
-    <col min="2" max="2" width="25.125" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -2349,75 +2349,75 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" t="s">
         <v>111</v>
-      </c>
-      <c r="B2" t="s">
-        <v>112</v>
       </c>
       <c r="C2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" t="s">
         <v>113</v>
-      </c>
-      <c r="B3" t="s">
-        <v>114</v>
       </c>
       <c r="C3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="3:3" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="3:3" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C29" s="2"/>
     </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C30" s="2"/>
     </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C33" s="2"/>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C34" s="2"/>
     </row>
   </sheetData>
@@ -2434,14 +2434,14 @@
       <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="18.875" customWidth="1"/>
-    <col min="5" max="5" width="27.375" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
     <col min="6" max="6" width="27" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>71</v>
       </c>
@@ -2537,13 +2537,13 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.375" customWidth="1"/>
-    <col min="2" max="2" width="34.875" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="115" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>91</v>
       </c>
@@ -2573,13 +2573,13 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.625" customWidth="1"/>
-    <col min="2" max="2" width="22.375" style="8" customWidth="1"/>
+    <col min="1" max="1" width="46.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -2587,42 +2587,42 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>100</v>
       </c>
@@ -2641,15 +2641,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.375" customWidth="1"/>
-    <col min="2" max="2" width="12.125" customWidth="1"/>
-    <col min="4" max="4" width="15.125" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -2690,14 +2690,14 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="9" style="7"/>
     <col min="5" max="5" width="14.5" customWidth="1"/>
     <col min="6" max="6" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -2756,17 +2756,17 @@
       <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="15.625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="13.625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="21.625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
     <col min="5" max="5" width="10.5" style="7"/>
-    <col min="6" max="6" width="17.375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
@@ -2786,7 +2786,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>80</v>
       </c>
@@ -2814,12 +2814,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -2861,17 +2861,17 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.125" customWidth="1"/>
-    <col min="2" max="2" width="23.875" customWidth="1"/>
-    <col min="3" max="3" width="22.625" customWidth="1"/>
-    <col min="4" max="4" width="24.125" customWidth="1"/>
-    <col min="5" max="5" width="23.875" customWidth="1"/>
-    <col min="8" max="8" width="53.625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" customWidth="1"/>
+    <col min="8" max="8" width="53.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>83</v>
       </c>
@@ -2915,22 +2915,22 @@
       </c>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G8" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating formatting of datasets and fixing erros associated with metadata
</commit_message>
<xml_diff>
--- a/data-raw/FISHBIO_submission/FISHBIO_PIT_detection_metadata.xlsx
+++ b/data-raw/FISHBIO_submission/FISHBIO_PIT_detection_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddeerubenson/Documents/git/fishbio-stanislaus-o.mykiss/data-raw/FISHBIO_submission/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddeerubenson/Documents/git/CVPIA/fishbio-stanislaus-o.mykiss/data-raw/FISHBIO_submission/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1CADFE7-E966-A646-B072-4E2B0A2D22DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5EF516B-2905-7F46-ACBD-FA405F58CDB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28520" windowHeight="15740" tabRatio="834" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36340" yWindow="1320" windowWidth="28520" windowHeight="15740" tabRatio="834" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -491,7 +491,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -521,6 +521,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1020,7 +1026,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N9" sqref="N9"/>
+      <selection pane="bottomLeft" activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1130,6 +1136,12 @@
       </c>
       <c r="L3" s="15" t="s">
         <v>87</v>
+      </c>
+      <c r="M3" s="17">
+        <v>0</v>
+      </c>
+      <c r="N3" s="18">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1022" ht="34" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added edits from Michael and changed all to lower case
</commit_message>
<xml_diff>
--- a/data-raw/FISHBIO_submission/FISHBIO_PIT_detection_metadata.xlsx
+++ b/data-raw/FISHBIO_submission/FISHBIO_PIT_detection_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddeerubenson/Documents/git/CVPIA/fishbio-stanislaus-o.mykiss/data-raw/FISHBIO_submission/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5EF516B-2905-7F46-ACBD-FA405F58CDB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A213C4B-D408-804F-AA53-CA4CB840628D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36340" yWindow="1320" windowWidth="28520" windowHeight="15740" tabRatio="834" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35060" yWindow="4160" windowWidth="28520" windowHeight="15740" tabRatio="834" firstSheet="5" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="attribute" sheetId="9" r:id="rId11"/>
     <sheet name="code_definitions" sheetId="10" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="130">
   <si>
     <t>first_name</t>
   </si>
@@ -386,9 +386,6 @@
     <t>enumerated</t>
   </si>
   <si>
-    <t xml:space="preserve">If species detected on multiple days (yes, no) </t>
-  </si>
-  <si>
     <t xml:space="preserve">Source of origional tag </t>
   </si>
   <si>
@@ -416,7 +413,19 @@
     <t>Any additional comments describing the passage record</t>
   </si>
   <si>
-    <t>RBT</t>
+    <t>rbt</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>If species detected on multiple days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If species detected on multiple days </t>
   </si>
 </sst>
 </file>
@@ -1024,9 +1033,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMH11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O14" sqref="O14"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1158,18 +1167,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:1022" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1022" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>88</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:1022" ht="34" x14ac:dyDescent="0.2">
@@ -1177,7 +1186,7 @@
         <v>105</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>88</v>
@@ -2223,7 +2232,7 @@
         <v>107</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>85</v>
@@ -2249,7 +2258,7 @@
         <v>108</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>88</v>
@@ -2263,23 +2272,23 @@
         <v>109</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="H10" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="G10" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="H10" s="6" t="s">
+      <c r="I10" s="15" t="s">
         <v>123</v>
-      </c>
-      <c r="I10" s="15" t="s">
-        <v>124</v>
       </c>
       <c r="J10" s="16"/>
       <c r="K10" s="15"/>
@@ -2296,7 +2305,7 @@
         <v>110</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="15" t="s">
@@ -2338,9 +2347,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2363,7 +2372,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
         <v>111</v>
@@ -2381,6 +2390,28 @@
       </c>
       <c r="C3" t="s">
         <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>